<commit_message>
change in US5 Acceptance Criteria
</commit_message>
<xml_diff>
--- a/features/RTM.xlsx
+++ b/features/RTM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gokarnabhandari/Documents/Revature Training/Assignments/Project 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gokarnabhandari/Documents/Revature Training/Assignments/Project 2/PlanetariumGroup/features/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB308843-0371-8D44-970C-4368BBC5F16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD38CB5A-9F40-914E-A01C-FAAF45AA72A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{F782749A-F44B-4770-ADC0-B107849E38C9}"/>
+    <workbookView xWindow="33600" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{F782749A-F44B-4770-ADC0-B107849E38C9}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="243">
   <si>
     <t>ID</t>
   </si>
@@ -2155,6 +2155,27 @@
   </si>
   <si>
     <t>Invalid moon name Alert</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">And </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>the user is in the home page</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2475,7 +2496,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2526,6 +2547,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2544,25 +2571,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2571,10 +2592,37 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2583,50 +2631,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -3092,7 +3107,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3274,7 +3289,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -3282,43 +3297,43 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="27"/>
+      <c r="A3" s="29"/>
       <c r="B3" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="27"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="27"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="27"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="27"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="11" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -3326,13 +3341,13 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="28"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="28" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -3340,25 +3355,25 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="27"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="27"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="28"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="13" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="28" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -3366,85 +3381,85 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="27"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="27"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="12" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="27"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="12" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="27"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="27"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="12" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="27"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="12" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="27"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="14" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="27"/>
+      <c r="A23" s="29"/>
       <c r="B23" s="14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="27"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="27"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="14" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="27"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="14" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="27"/>
+      <c r="A27" s="29"/>
       <c r="B27" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="28"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="13" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="28" t="s">
         <v>11</v>
       </c>
       <c r="B29" s="7" t="s">
@@ -3452,19 +3467,19 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="27"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="27"/>
+      <c r="A31" s="29"/>
       <c r="B31" s="14" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="28"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="13" t="s">
         <v>56</v>
       </c>
@@ -3513,10 +3528,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="31" t="s">
         <v>69</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -3525,8 +3540,8 @@
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="31"/>
-      <c r="B3" s="29"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="31"/>
       <c r="C3" s="1" t="s">
         <v>62</v>
       </c>
@@ -3535,43 +3550,43 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="31"/>
-      <c r="B4" s="29"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="31"/>
-      <c r="B5" s="29"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="31"/>
-      <c r="B6" s="29"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="31"/>
-      <c r="B7" s="29"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="31"/>
-      <c r="B8" s="29"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="31"/>
-      <c r="B9" s="30" t="s">
+      <c r="A9" s="33"/>
+      <c r="B9" s="32" t="s">
         <v>70</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -3579,36 +3594,36 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="31"/>
-      <c r="B10" s="30"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="31"/>
-      <c r="B11" s="30"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="32"/>
       <c r="C11" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="31"/>
-      <c r="B12" s="30"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" s="31"/>
-      <c r="B13" s="30"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="31"/>
-      <c r="B14" s="30"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="1" t="s">
         <v>74</v>
       </c>
@@ -3630,7 +3645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F9112B-A9DE-E441-995E-55E1682CB647}">
   <dimension ref="A1:F176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A131" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B177" sqref="B177"/>
     </sheetView>
   </sheetViews>
@@ -3645,28 +3660,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="32" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="29" t="s">
+      <c r="B2" s="31"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
@@ -3733,16 +3748,16 @@
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="30" t="s">
+      <c r="B7" s="32"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
@@ -3834,11 +3849,11 @@
       <c r="C12" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -4009,11 +4024,11 @@
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="34"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="37"/>
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
@@ -4178,20 +4193,20 @@
       <c r="F37" s="20"/>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="32" t="s">
+      <c r="A38" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
     </row>
     <row r="39" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="38" t="s">
+      <c r="A39" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="B39" s="38"/>
+      <c r="B39" s="36"/>
       <c r="C39" s="24"/>
-      <c r="D39" s="52" t="s">
+      <c r="D39" s="43" t="s">
         <v>222</v>
       </c>
     </row>
@@ -4202,7 +4217,7 @@
       <c r="B40" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="D40" s="52"/>
+      <c r="D40" s="43"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
@@ -4211,17 +4226,17 @@
       <c r="B41" t="s">
         <v>151</v>
       </c>
-      <c r="D41" s="52"/>
+      <c r="D41" s="43"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D42" s="52"/>
+      <c r="D42" s="43"/>
     </row>
     <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="38" t="s">
+      <c r="A43" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="B43" s="38"/>
-      <c r="D43" s="52"/>
+      <c r="B43" s="36"/>
+      <c r="D43" s="43"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="21" t="s">
@@ -4230,7 +4245,7 @@
       <c r="B44" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="D44" s="52"/>
+      <c r="D44" s="43"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
@@ -4239,18 +4254,18 @@
       <c r="B45" t="s">
         <v>151</v>
       </c>
-      <c r="D45" s="52"/>
+      <c r="D45" s="43"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D46" s="52"/>
+      <c r="D46" s="43"/>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="38" t="s">
+      <c r="A47" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="B47" s="38"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="52"/>
+      <c r="B47" s="36"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="43"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="21" t="s">
@@ -4262,7 +4277,7 @@
       <c r="C48" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="D48" s="52"/>
+      <c r="D48" s="43"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
@@ -4274,13 +4289,13 @@
       <c r="C49" t="s">
         <v>151</v>
       </c>
-      <c r="D49" s="52"/>
+      <c r="D49" s="43"/>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="29" t="s">
+      <c r="A52" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="B52" s="29"/>
+      <c r="B52" s="31"/>
       <c r="C52" s="17"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -4301,10 +4316,10 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="29" t="s">
+      <c r="A56" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="B56" s="29"/>
+      <c r="B56" s="31"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
@@ -4379,11 +4394,11 @@
       </c>
     </row>
     <row r="67" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="30" t="s">
+      <c r="A67" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="B67" s="30"/>
-      <c r="C67" s="37"/>
+      <c r="B67" s="32"/>
+      <c r="C67" s="34"/>
     </row>
     <row r="68" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="19" t="s">
@@ -4450,11 +4465,11 @@
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="30" t="s">
+      <c r="A75" s="32" t="s">
         <v>185</v>
       </c>
-      <c r="B75" s="30"/>
-      <c r="C75" s="37"/>
+      <c r="B75" s="32"/>
+      <c r="C75" s="34"/>
     </row>
     <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="19" t="s">
@@ -4564,11 +4579,11 @@
       <c r="C86" s="2"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="33" t="s">
+      <c r="A87" s="35" t="s">
         <v>193</v>
       </c>
-      <c r="B87" s="33"/>
-      <c r="C87" s="34"/>
+      <c r="B87" s="35"/>
+      <c r="C87" s="37"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="21" t="s">
@@ -4791,12 +4806,12 @@
       </c>
     </row>
     <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="33" t="s">
+      <c r="A109" s="35" t="s">
         <v>200</v>
       </c>
-      <c r="B109" s="33"/>
-      <c r="C109" s="33"/>
-      <c r="D109" s="33"/>
+      <c r="B109" s="35"/>
+      <c r="C109" s="35"/>
+      <c r="D109" s="35"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="21" t="s">
@@ -5127,18 +5142,18 @@
       <c r="D134" s="20"/>
     </row>
     <row r="135" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="32" t="s">
+      <c r="A135" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B135" s="32"/>
-      <c r="C135" s="32"/>
+      <c r="B135" s="38"/>
+      <c r="C135" s="38"/>
       <c r="D135" s="2"/>
     </row>
     <row r="136" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A136" s="38" t="s">
+      <c r="A136" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="B136" s="38"/>
+      <c r="B136" s="36"/>
       <c r="C136" s="24"/>
       <c r="D136" s="24"/>
     </row>
@@ -5159,10 +5174,10 @@
       </c>
     </row>
     <row r="140" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A140" s="38" t="s">
+      <c r="A140" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="B140" s="38"/>
+      <c r="B140" s="36"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="21" t="s">
@@ -5181,11 +5196,11 @@
       </c>
     </row>
     <row r="144" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A144" s="38" t="s">
+      <c r="A144" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="B144" s="38"/>
-      <c r="C144" s="38"/>
+      <c r="B144" s="36"/>
+      <c r="C144" s="36"/>
       <c r="D144" s="24"/>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
@@ -5211,11 +5226,11 @@
       </c>
     </row>
     <row r="148" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A148" s="38" t="s">
+      <c r="A148" s="36" t="s">
         <v>199</v>
       </c>
-      <c r="B148" s="38"/>
-      <c r="C148" s="38"/>
+      <c r="B148" s="36"/>
+      <c r="C148" s="36"/>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="21" t="s">
@@ -5240,10 +5255,10 @@
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A152" s="29" t="s">
+      <c r="A152" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="B152" s="29"/>
+      <c r="B152" s="31"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="21" t="s">
@@ -5262,10 +5277,10 @@
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A156" s="29" t="s">
+      <c r="A156" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="B156" s="29"/>
+      <c r="B156" s="31"/>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="21" t="s">
@@ -5284,11 +5299,11 @@
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A160" s="30" t="s">
+      <c r="A160" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="B160" s="30"/>
-      <c r="C160" s="37"/>
+      <c r="B160" s="32"/>
+      <c r="C160" s="34"/>
     </row>
     <row r="161" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A161" s="19" t="s">
@@ -5313,11 +5328,11 @@
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A164" s="30" t="s">
+      <c r="A164" s="32" t="s">
         <v>185</v>
       </c>
-      <c r="B164" s="30"/>
-      <c r="C164" s="37"/>
+      <c r="B164" s="32"/>
+      <c r="C164" s="34"/>
     </row>
     <row r="165" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A165" s="19" t="s">
@@ -5347,11 +5362,11 @@
       <c r="C167" s="17"/>
     </row>
     <row r="168" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="33" t="s">
+      <c r="A168" s="35" t="s">
         <v>193</v>
       </c>
-      <c r="B168" s="33"/>
-      <c r="C168" s="34"/>
+      <c r="B168" s="35"/>
+      <c r="C168" s="37"/>
     </row>
     <row r="169" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="19" t="s">
@@ -5384,10 +5399,10 @@
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A173" s="33" t="s">
+      <c r="A173" s="35" t="s">
         <v>200</v>
       </c>
-      <c r="B173" s="33"/>
+      <c r="B173" s="35"/>
     </row>
     <row r="174" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A174" s="19" t="s">
@@ -5415,27 +5430,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A164:C164"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="A144:C144"/>
-    <mergeCell ref="A148:C148"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="A156:B156"/>
-    <mergeCell ref="A168:C168"/>
-    <mergeCell ref="A135:C135"/>
-    <mergeCell ref="A160:C160"/>
-    <mergeCell ref="A87:C87"/>
-    <mergeCell ref="A109:D109"/>
-    <mergeCell ref="A136:B136"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="A75:C75"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A83:C83"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A56:B56"/>
     <mergeCell ref="A38:D38"/>
     <mergeCell ref="A52:B52"/>
     <mergeCell ref="A22:C22"/>
@@ -5447,6 +5441,27 @@
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D39:D49"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A83:C83"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="A160:C160"/>
+    <mergeCell ref="A87:C87"/>
+    <mergeCell ref="A109:D109"/>
+    <mergeCell ref="A136:B136"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="A164:C164"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A144:C144"/>
+    <mergeCell ref="A148:C148"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="A156:B156"/>
+    <mergeCell ref="A168:C168"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5458,9 +5473,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14EEDEC-6C50-4FA1-BB35-C40D70D716CC}">
   <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5490,10 +5505,10 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="45" t="s">
         <v>69</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -5506,8 +5521,8 @@
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="31"/>
-      <c r="B3" s="41"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="45"/>
       <c r="C3" s="1" t="s">
         <v>62</v>
       </c>
@@ -5517,48 +5532,48 @@
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="31"/>
-      <c r="B4" s="41"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="45"/>
       <c r="C4" s="1" t="s">
         <v>206</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="31"/>
-      <c r="B5" s="41"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="45"/>
       <c r="C5" s="1" t="s">
         <v>79</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="31"/>
-      <c r="B6" s="41"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="1" t="s">
         <v>65</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="31"/>
-      <c r="B7" s="41"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="1" t="s">
         <v>205</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="31"/>
-      <c r="B8" s="42"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="46"/>
       <c r="C8" s="1" t="s">
         <v>67</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="31"/>
-      <c r="B9" s="43" t="s">
+      <c r="A9" s="33"/>
+      <c r="B9" s="52" t="s">
         <v>70</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -5566,57 +5581,57 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="31"/>
-      <c r="B10" s="30"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="31"/>
-      <c r="B11" s="30"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="32"/>
       <c r="C11" s="1" t="s">
         <v>206</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="31"/>
-      <c r="B12" s="30"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="1" t="s">
         <v>79</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="31"/>
-      <c r="B13" s="30"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="1" t="s">
         <v>65</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="31"/>
-      <c r="B14" s="30"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="1" t="s">
         <v>80</v>
       </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" s="31"/>
-      <c r="B15" s="44"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="53"/>
       <c r="C15" s="1" t="s">
         <v>74</v>
       </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="44" t="s">
         <v>69</v>
       </c>
       <c r="C16" s="15" t="s">
@@ -5626,8 +5641,8 @@
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="31"/>
-      <c r="B17" s="41"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="45"/>
       <c r="C17" s="1" t="s">
         <v>206</v>
       </c>
@@ -5635,8 +5650,8 @@
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="31"/>
-      <c r="B18" s="41"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="45"/>
       <c r="C18" s="1" t="s">
         <v>79</v>
       </c>
@@ -5644,8 +5659,8 @@
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="31"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="15" t="s">
         <v>209</v>
       </c>
@@ -5653,8 +5668,8 @@
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A20" s="31"/>
-      <c r="B20" s="42"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="46"/>
       <c r="C20" s="15" t="s">
         <v>87</v>
       </c>
@@ -5662,8 +5677,8 @@
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="31"/>
-      <c r="B21" s="43" t="s">
+      <c r="A21" s="33"/>
+      <c r="B21" s="52" t="s">
         <v>70</v>
       </c>
       <c r="C21" s="15" t="s">
@@ -5673,8 +5688,8 @@
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A22" s="31"/>
-      <c r="B22" s="30"/>
+      <c r="A22" s="33"/>
+      <c r="B22" s="32"/>
       <c r="C22" s="15" t="s">
         <v>210</v>
       </c>
@@ -5682,8 +5697,8 @@
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="31"/>
-      <c r="B23" s="30"/>
+      <c r="A23" s="33"/>
+      <c r="B23" s="32"/>
       <c r="C23" s="15" t="s">
         <v>88</v>
       </c>
@@ -5691,58 +5706,58 @@
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="31"/>
-      <c r="B24" s="30"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="32"/>
       <c r="C24" s="15" t="s">
         <v>211</v>
       </c>
       <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A25" s="31"/>
-      <c r="B25" s="30"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="32"/>
       <c r="C25" s="15" t="s">
         <v>89</v>
       </c>
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="31"/>
-      <c r="B26" s="44"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="53"/>
       <c r="C26" s="15" t="s">
         <v>90</v>
       </c>
       <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="45" t="s">
+      <c r="B27" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="49" t="s">
+      <c r="C27" s="51" t="s">
         <v>212</v>
       </c>
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="31"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="49"/>
+      <c r="A28" s="33"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="51"/>
       <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A29" s="31"/>
-      <c r="B29" s="42"/>
+      <c r="A29" s="33"/>
+      <c r="B29" s="46"/>
       <c r="C29" s="15" t="s">
         <v>213</v>
       </c>
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="31"/>
-      <c r="B30" s="43" t="s">
+      <c r="A30" s="33"/>
+      <c r="B30" s="52" t="s">
         <v>70</v>
       </c>
       <c r="C30" s="16" t="s">
@@ -5751,26 +5766,26 @@
       <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A31" s="31"/>
-      <c r="B31" s="30"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="32"/>
       <c r="C31" s="16" t="s">
         <v>92</v>
       </c>
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="31"/>
-      <c r="B32" s="44"/>
+      <c r="A32" s="33"/>
+      <c r="B32" s="53"/>
       <c r="C32" s="16" t="s">
         <v>93</v>
       </c>
       <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="45" t="s">
+      <c r="B33" s="44" t="s">
         <v>69</v>
       </c>
       <c r="C33" s="15" t="s">
@@ -5779,115 +5794,115 @@
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="31"/>
-      <c r="B34" s="51"/>
+      <c r="A34" s="33"/>
+      <c r="B34" s="45"/>
       <c r="C34" s="15" t="s">
         <v>214</v>
       </c>
       <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A35" s="31"/>
-      <c r="B35" s="51"/>
+      <c r="A35" s="33"/>
+      <c r="B35" s="45"/>
       <c r="C35" s="15" t="s">
         <v>215</v>
       </c>
       <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A36" s="31"/>
-      <c r="B36" s="51"/>
+      <c r="A36" s="33"/>
+      <c r="B36" s="45"/>
       <c r="C36" s="15" t="s">
         <v>216</v>
       </c>
       <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="31"/>
-      <c r="B37" s="51"/>
+      <c r="A37" s="33"/>
+      <c r="B37" s="45"/>
       <c r="C37" s="15" t="s">
         <v>217</v>
       </c>
       <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="31"/>
-      <c r="B38" s="51"/>
+      <c r="A38" s="33"/>
+      <c r="B38" s="45"/>
       <c r="C38" s="15" t="s">
         <v>218</v>
       </c>
       <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A39" s="31"/>
-      <c r="B39" s="42"/>
+      <c r="A39" s="33"/>
+      <c r="B39" s="46"/>
       <c r="C39" s="15" t="s">
         <v>219</v>
       </c>
       <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A40" s="31"/>
-      <c r="B40" s="43" t="s">
+      <c r="A40" s="33"/>
+      <c r="B40" s="52" t="s">
         <v>70</v>
       </c>
       <c r="C40" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="D40" s="55" t="s">
+      <c r="D40" s="26" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="31"/>
-      <c r="B41" s="50"/>
+      <c r="A41" s="33"/>
+      <c r="B41" s="32"/>
       <c r="C41" s="15" t="s">
         <v>212</v>
       </c>
       <c r="D41" s="15"/>
     </row>
     <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="31"/>
-      <c r="B42" s="50"/>
+      <c r="A42" s="33"/>
+      <c r="B42" s="32"/>
       <c r="C42" s="15" t="s">
         <v>214</v>
       </c>
       <c r="D42" s="15"/>
     </row>
     <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A43" s="31"/>
-      <c r="B43" s="50"/>
+      <c r="A43" s="33"/>
+      <c r="B43" s="32"/>
       <c r="C43" s="15" t="s">
         <v>215</v>
       </c>
       <c r="D43" s="15"/>
     </row>
     <row r="44" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A44" s="31"/>
-      <c r="B44" s="50"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="32"/>
       <c r="C44" s="15" t="s">
         <v>216</v>
       </c>
       <c r="D44" s="15"/>
     </row>
     <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="31"/>
-      <c r="B45" s="50"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="32"/>
       <c r="C45" s="15" t="s">
         <v>217</v>
       </c>
       <c r="D45" s="15"/>
     </row>
     <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A46" s="31"/>
-      <c r="B46" s="44"/>
+      <c r="A46" s="33"/>
+      <c r="B46" s="53"/>
       <c r="C46" s="15" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="31"/>
-      <c r="B47" s="45" t="s">
+      <c r="A47" s="33"/>
+      <c r="B47" s="44" t="s">
         <v>69</v>
       </c>
       <c r="C47" s="15" t="s">
@@ -5896,132 +5911,132 @@
       <c r="D47" s="4"/>
     </row>
     <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="31"/>
-      <c r="B48" s="51"/>
+      <c r="A48" s="33"/>
+      <c r="B48" s="45"/>
       <c r="C48" s="15" t="s">
         <v>225</v>
       </c>
       <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A49" s="31"/>
-      <c r="B49" s="51"/>
+      <c r="A49" s="33"/>
+      <c r="B49" s="45"/>
       <c r="C49" s="15" t="s">
         <v>226</v>
       </c>
       <c r="D49" s="4"/>
     </row>
     <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="31"/>
-      <c r="B50" s="51"/>
+      <c r="A50" s="33"/>
+      <c r="B50" s="45"/>
       <c r="C50" s="15" t="s">
         <v>238</v>
       </c>
       <c r="D50" s="4"/>
     </row>
     <row r="51" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A51" s="31"/>
-      <c r="B51" s="51"/>
+      <c r="A51" s="33"/>
+      <c r="B51" s="45"/>
       <c r="C51" s="15" t="s">
         <v>227</v>
       </c>
       <c r="D51" s="4"/>
     </row>
     <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="31"/>
-      <c r="B52" s="51"/>
+      <c r="A52" s="33"/>
+      <c r="B52" s="45"/>
       <c r="C52" s="15" t="s">
         <v>228</v>
       </c>
-      <c r="D52" s="56"/>
+      <c r="D52" s="27"/>
     </row>
     <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="31"/>
-      <c r="B53" s="51"/>
+      <c r="A53" s="33"/>
+      <c r="B53" s="45"/>
       <c r="C53" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="D53" s="56"/>
+      <c r="D53" s="27"/>
     </row>
     <row r="54" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A54" s="31"/>
-      <c r="B54" s="42"/>
+      <c r="A54" s="33"/>
+      <c r="B54" s="46"/>
       <c r="C54" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="D54" s="56"/>
+      <c r="D54" s="27"/>
     </row>
     <row r="55" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A55" s="31"/>
-      <c r="B55" s="53" t="s">
+      <c r="A55" s="33"/>
+      <c r="B55" s="47" t="s">
         <v>70</v>
       </c>
       <c r="C55" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="D55" s="56"/>
+      <c r="D55" s="27"/>
     </row>
     <row r="56" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="31"/>
-      <c r="B56" s="54"/>
+      <c r="A56" s="33"/>
+      <c r="B56" s="48"/>
       <c r="C56" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="D56" s="56"/>
+        <v>242</v>
+      </c>
+      <c r="D56" s="27"/>
     </row>
     <row r="57" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A57" s="31"/>
-      <c r="B57" s="54"/>
+      <c r="A57" s="33"/>
+      <c r="B57" s="48"/>
       <c r="C57" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="D57" s="56"/>
+      <c r="D57" s="27"/>
     </row>
     <row r="58" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A58" s="31"/>
-      <c r="B58" s="54"/>
+      <c r="A58" s="33"/>
+      <c r="B58" s="48"/>
       <c r="C58" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="D58" s="56"/>
+      <c r="D58" s="27"/>
     </row>
     <row r="59" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="31"/>
-      <c r="B59" s="54"/>
+      <c r="A59" s="33"/>
+      <c r="B59" s="48"/>
       <c r="C59" s="15" t="s">
         <v>238</v>
       </c>
-      <c r="D59" s="56"/>
+      <c r="D59" s="27"/>
     </row>
     <row r="60" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A60" s="31"/>
-      <c r="B60" s="54"/>
+      <c r="A60" s="33"/>
+      <c r="B60" s="48"/>
       <c r="C60" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="D60" s="56"/>
+      <c r="D60" s="27"/>
     </row>
     <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="31"/>
-      <c r="B61" s="54"/>
+      <c r="A61" s="33"/>
+      <c r="B61" s="48"/>
       <c r="C61" s="15" t="s">
         <v>228</v>
       </c>
-      <c r="D61" s="56"/>
+      <c r="D61" s="27"/>
     </row>
     <row r="62" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A62" s="31"/>
-      <c r="B62" s="54"/>
+      <c r="A62" s="33"/>
+      <c r="B62" s="48"/>
       <c r="C62" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="D62" s="56"/>
+      <c r="D62" s="27"/>
     </row>
     <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="31" t="s">
+      <c r="A63" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="B63" s="45" t="s">
+      <c r="B63" s="44" t="s">
         <v>69</v>
       </c>
       <c r="C63" s="15" t="s">
@@ -6030,56 +6045,56 @@
       <c r="D63" s="4"/>
     </row>
     <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="31"/>
-      <c r="B64" s="51"/>
+      <c r="A64" s="33"/>
+      <c r="B64" s="54"/>
       <c r="C64" s="15" t="s">
         <v>214</v>
       </c>
       <c r="D64" s="4"/>
     </row>
     <row r="65" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A65" s="31"/>
-      <c r="B65" s="51"/>
+      <c r="A65" s="33"/>
+      <c r="B65" s="54"/>
       <c r="C65" s="15" t="s">
         <v>234</v>
       </c>
       <c r="D65" s="4"/>
     </row>
     <row r="66" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" s="31"/>
-      <c r="B66" s="51"/>
+      <c r="A66" s="33"/>
+      <c r="B66" s="54"/>
       <c r="C66" s="15" t="s">
         <v>232</v>
       </c>
       <c r="D66" s="4"/>
     </row>
     <row r="67" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="31"/>
-      <c r="B67" s="51"/>
+      <c r="A67" s="33"/>
+      <c r="B67" s="54"/>
       <c r="C67" s="15" t="s">
         <v>218</v>
       </c>
       <c r="D67" s="4"/>
     </row>
     <row r="68" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="31"/>
-      <c r="B68" s="51"/>
+      <c r="A68" s="33"/>
+      <c r="B68" s="54"/>
       <c r="C68" s="15" t="s">
         <v>236</v>
       </c>
       <c r="D68" s="4"/>
     </row>
     <row r="69" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A69" s="31"/>
-      <c r="B69" s="42"/>
+      <c r="A69" s="33"/>
+      <c r="B69" s="46"/>
       <c r="C69" s="15" t="s">
         <v>233</v>
       </c>
       <c r="D69" s="4"/>
     </row>
     <row r="70" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A70" s="31"/>
-      <c r="B70" s="45" t="s">
+      <c r="A70" s="33"/>
+      <c r="B70" s="44" t="s">
         <v>69</v>
       </c>
       <c r="C70" s="15" t="s">
@@ -6088,169 +6103,168 @@
       <c r="D70" s="4"/>
     </row>
     <row r="71" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A71" s="31"/>
-      <c r="B71" s="51"/>
+      <c r="A71" s="33"/>
+      <c r="B71" s="54"/>
       <c r="C71" s="15" t="s">
         <v>214</v>
       </c>
       <c r="D71" s="4"/>
     </row>
     <row r="72" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A72" s="31"/>
-      <c r="B72" s="51"/>
+      <c r="A72" s="33"/>
+      <c r="B72" s="54"/>
       <c r="C72" s="15" t="s">
         <v>234</v>
       </c>
       <c r="D72" s="4"/>
     </row>
     <row r="73" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A73" s="31"/>
-      <c r="B73" s="51"/>
+      <c r="A73" s="33"/>
+      <c r="B73" s="54"/>
       <c r="C73" s="15" t="s">
         <v>232</v>
       </c>
       <c r="D73" s="4"/>
     </row>
     <row r="74" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A74" s="31"/>
-      <c r="B74" s="51"/>
+      <c r="A74" s="33"/>
+      <c r="B74" s="54"/>
       <c r="C74" s="15" t="s">
         <v>218</v>
       </c>
       <c r="D74" s="4"/>
     </row>
     <row r="75" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="31"/>
-      <c r="B75" s="42"/>
+      <c r="A75" s="33"/>
+      <c r="B75" s="46"/>
       <c r="C75" s="15" t="s">
         <v>235</v>
       </c>
       <c r="D75" s="4"/>
     </row>
-    <row r="76" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A76" s="31"/>
-      <c r="B76" s="46" t="s">
+    <row r="76" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A76" s="33"/>
+      <c r="B76" s="49" t="s">
         <v>70</v>
       </c>
       <c r="C76" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="D76" s="4"/>
+    </row>
+    <row r="77" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A77" s="33"/>
+      <c r="B77" s="55"/>
+      <c r="C77" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="D76" s="4"/>
-    </row>
-    <row r="77" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" s="31"/>
-      <c r="B77" s="47"/>
-      <c r="C77" s="15" t="s">
+      <c r="D77" s="4"/>
+    </row>
+    <row r="78" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A78" s="33"/>
+      <c r="B78" s="55"/>
+      <c r="C78" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="D77" s="4"/>
-    </row>
-    <row r="78" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A78" s="31"/>
-      <c r="B78" s="47"/>
-      <c r="C78" s="15" t="s">
+      <c r="D78" s="4"/>
+    </row>
+    <row r="79" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A79" s="33"/>
+      <c r="B79" s="55"/>
+      <c r="C79" s="15" t="s">
         <v>234</v>
       </c>
-      <c r="D78" s="4"/>
-    </row>
-    <row r="79" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="31"/>
-      <c r="B79" s="47"/>
-      <c r="C79" s="15" t="s">
+      <c r="D79" s="4"/>
+    </row>
+    <row r="80" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A80" s="33"/>
+      <c r="B80" s="55"/>
+      <c r="C80" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="D79" s="4"/>
-    </row>
-    <row r="80" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A80" s="31"/>
-      <c r="B80" s="48"/>
-      <c r="C80" s="15" t="s">
+      <c r="D80" s="4"/>
+    </row>
+    <row r="81" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A81" s="33"/>
+      <c r="B81" s="50"/>
+      <c r="C81" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="D80" s="4"/>
-    </row>
-    <row r="81" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A81" s="31"/>
-      <c r="B81" s="46" t="s">
+      <c r="D81" s="4"/>
+    </row>
+    <row r="82" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A82" s="33"/>
+      <c r="B82" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="C81" s="15" t="s">
+      <c r="C82" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="D82" s="4"/>
+    </row>
+    <row r="83" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A83" s="33"/>
+      <c r="B83" s="55"/>
+      <c r="C83" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="D81" s="4"/>
-    </row>
-    <row r="82" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A82" s="31"/>
-      <c r="B82" s="47"/>
-      <c r="C82" s="15" t="s">
+      <c r="D83" s="4"/>
+    </row>
+    <row r="84" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A84" s="33"/>
+      <c r="B84" s="55"/>
+      <c r="C84" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="D82" s="4"/>
-    </row>
-    <row r="83" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A83" s="31"/>
-      <c r="B83" s="47"/>
-      <c r="C83" s="15" t="s">
+      <c r="D84" s="4"/>
+    </row>
+    <row r="85" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A85" s="33"/>
+      <c r="B85" s="55"/>
+      <c r="C85" s="15" t="s">
         <v>237</v>
       </c>
-      <c r="D83" s="4"/>
-    </row>
-    <row r="84" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A84" s="31"/>
-      <c r="B84" s="47"/>
-      <c r="C84" s="15" t="s">
+      <c r="D85" s="4"/>
+    </row>
+    <row r="86" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A86" s="2"/>
+      <c r="B86" s="55"/>
+      <c r="C86" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="D84" s="4"/>
-    </row>
-    <row r="85" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A85" s="31"/>
-      <c r="B85" s="48"/>
-      <c r="C85" s="15" t="s">
+      <c r="D86" s="4"/>
+    </row>
+    <row r="87" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A87" s="2"/>
+      <c r="B87" s="50"/>
+      <c r="C87" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="D85" s="4"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="2"/>
-      <c r="B86" s="57"/>
-      <c r="C86" s="15"/>
-      <c r="D86" s="4"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="2"/>
-      <c r="B87" s="58"/>
-      <c r="C87" s="15"/>
       <c r="D87" s="4"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
-      <c r="B88" s="58"/>
-      <c r="C88" s="15"/>
+      <c r="B88" s="56"/>
       <c r="D88" s="4"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="2"/>
-      <c r="B89" s="58"/>
-      <c r="C89" s="15"/>
+      <c r="B89" s="56"/>
       <c r="D89" s="4"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
-      <c r="B90" s="59"/>
-      <c r="C90" s="15"/>
+      <c r="B90" s="57"/>
       <c r="D90" s="4"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
       <c r="D91" s="4"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
       <c r="D92" s="4"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -6341,17 +6355,7 @@
       <c r="C107" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="B47:B54"/>
-    <mergeCell ref="B55:B62"/>
-    <mergeCell ref="B63:B69"/>
-    <mergeCell ref="B70:B75"/>
-    <mergeCell ref="B76:B80"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="B33:B39"/>
-    <mergeCell ref="B40:B46"/>
-    <mergeCell ref="B81:B85"/>
-    <mergeCell ref="B86:B90"/>
+  <mergeCells count="20">
     <mergeCell ref="A63:A85"/>
     <mergeCell ref="A2:A15"/>
     <mergeCell ref="B2:B8"/>
@@ -6363,6 +6367,15 @@
     <mergeCell ref="A27:A32"/>
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B76:B81"/>
+    <mergeCell ref="B82:B87"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="B33:B39"/>
+    <mergeCell ref="B40:B46"/>
+    <mergeCell ref="B47:B54"/>
+    <mergeCell ref="B55:B62"/>
+    <mergeCell ref="B63:B69"/>
+    <mergeCell ref="B70:B75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -6404,7 +6417,7 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="31" t="s">
         <v>69</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -6415,43 +6428,43 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B3" s="29"/>
+      <c r="B3" s="31"/>
       <c r="C3" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B4" s="29"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B5" s="29"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B6" s="29"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B7" s="29"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B8" s="29"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="32" t="s">
         <v>70</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -6459,43 +6472,43 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B10" s="30"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B11" s="30"/>
+      <c r="B11" s="32"/>
       <c r="C11" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B12" s="30"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B13" s="30"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B14" s="30"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B15" s="30"/>
+      <c r="B15" s="32"/>
       <c r="C15" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="32" t="s">
         <v>70</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -6503,43 +6516,43 @@
       </c>
     </row>
     <row r="17" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B17" s="30"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B18" s="30"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B19" s="30"/>
+      <c r="B19" s="32"/>
       <c r="C19" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B20" s="30"/>
+      <c r="B20" s="32"/>
       <c r="C20" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="B21" s="30"/>
+      <c r="B21" s="32"/>
       <c r="C21" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="B22" s="30"/>
+      <c r="B22" s="32"/>
       <c r="C22" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="32" t="s">
         <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -6547,37 +6560,37 @@
       </c>
     </row>
     <row r="24" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B24" s="30"/>
+      <c r="B24" s="32"/>
       <c r="C24" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B25" s="30"/>
+      <c r="B25" s="32"/>
       <c r="C25" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B26" s="30"/>
+      <c r="B26" s="32"/>
       <c r="C26" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B27" s="30"/>
+      <c r="B27" s="32"/>
       <c r="C27" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="B28" s="30"/>
+      <c r="B28" s="32"/>
       <c r="C28" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="B29" s="30"/>
+      <c r="B29" s="32"/>
       <c r="C29" s="1" t="s">
         <v>74</v>
       </c>

</xml_diff>